<commit_message>
correcciones en reglas del documento stock actual
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_06_13022026_deco_exterior.xlsx
+++ b/data/output/Pedido_Semana_06_13022026_deco_exterior.xlsx
@@ -678,7 +678,7 @@
         </is>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>9203010004</t>
@@ -737,10 +737,10 @@
       </c>
       <c r="O3" s="7" t="inlineStr"/>
       <c r="P3" s="3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q3" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R3" s="2" t="n">
         <v>0</v>
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="U3" s="8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1119,10 +1119,10 @@
         <v>0</v>
       </c>
       <c r="M8" s="6" t="n">
-        <v>6.8</v>
+        <v>3.4</v>
       </c>
       <c r="N8" s="4" t="n">
-        <v>4.08</v>
+        <v>2.04</v>
       </c>
       <c r="O8" s="7" t="inlineStr">
         <is>
@@ -1130,10 +1130,10 @@
         </is>
       </c>
       <c r="P8" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q8" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R8" s="2" t="n">
         <v>0</v>
@@ -1145,10 +1145,10 @@
         <v>0</v>
       </c>
       <c r="U8" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" hidden="1">
       <c r="A9" s="2" t="inlineStr">
         <is>
           <t>9401010010</t>
@@ -1197,13 +1197,13 @@
         <v>1</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="6" t="n">
-        <v>7.95</v>
+        <v>0</v>
       </c>
       <c r="N9" s="4" t="n">
-        <v>4.77</v>
+        <v>0</v>
       </c>
       <c r="O9" s="7" t="inlineStr">
         <is>
@@ -1211,10 +1211,10 @@
         </is>
       </c>
       <c r="P9" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q9" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R9" s="2" t="n">
         <v>0</v>
@@ -1226,10 +1226,10 @@
         <v>1</v>
       </c>
       <c r="U9" s="8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" hidden="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
           <t>9401010025</t>
@@ -1242,7 +1242,7 @@
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">35CM     </t>
+          <t xml:space="preserve">11CM     </t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -1259,32 +1259,32 @@
         <v>1</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>5.98</v>
+        <v>0.58</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>2.39</v>
+        <v>0.23</v>
       </c>
       <c r="I10" s="5" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>C</t>
         </is>
       </c>
       <c r="J10" s="2" t="inlineStr">
         <is>
-          <t>REDUCIR 19%</t>
+          <t>REDUCIR 40%</t>
         </is>
       </c>
       <c r="K10" s="3" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="6" t="n">
-        <v>11.95</v>
+        <v>0</v>
       </c>
       <c r="N10" s="4" t="n">
-        <v>7.17</v>
+        <v>0</v>
       </c>
       <c r="O10" s="7" t="inlineStr">
         <is>
@@ -1292,25 +1292,25 @@
         </is>
       </c>
       <c r="P10" s="3" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R10" s="2" t="n">
         <v>0</v>
       </c>
       <c r="S10" s="2" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="T10" s="3" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="U10" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" hidden="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
           <t>9401010025</t>
@@ -1362,10 +1362,10 @@
         <v>0</v>
       </c>
       <c r="M11" s="6" t="n">
-        <v>5.45</v>
+        <v>0</v>
       </c>
       <c r="N11" s="4" t="n">
-        <v>3.27</v>
+        <v>0</v>
       </c>
       <c r="O11" s="7" t="inlineStr">
         <is>
@@ -1373,10 +1373,10 @@
         </is>
       </c>
       <c r="P11" s="3" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q11" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R11" s="2" t="n">
         <v>0</v>
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="U11" s="8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" hidden="1">
@@ -1404,7 +1404,7 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">11CM     </t>
+          <t xml:space="preserve">35CM     </t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr">
@@ -1421,19 +1421,19 @@
         <v>1</v>
       </c>
       <c r="G12" s="4" t="n">
-        <v>0.58</v>
+        <v>5.98</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>0.23</v>
+        <v>2.39</v>
       </c>
       <c r="I12" s="5" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>A</t>
         </is>
       </c>
       <c r="J12" s="2" t="inlineStr">
         <is>
-          <t>REDUCIR 40%</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K12" s="3" t="n">
@@ -1454,7 +1454,7 @@
         </is>
       </c>
       <c r="P12" s="3" t="n">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="Q12" s="3" t="n">
         <v>0</v>
@@ -1463,10 +1463,10 @@
         <v>0</v>
       </c>
       <c r="S12" s="2" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="T12" s="3" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="U12" s="8" t="n">
         <v>0</v>
@@ -1634,7 +1634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
           <t>9401020010</t>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">26CM     </t>
+          <t xml:space="preserve">15CM     </t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
@@ -1664,10 +1664,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="4" t="n">
-        <v>1.25</v>
+        <v>0.58</v>
       </c>
       <c r="H15" s="4" t="n">
-        <v>0.5</v>
+        <v>0.23</v>
       </c>
       <c r="I15" s="5" t="inlineStr">
         <is>
@@ -1676,20 +1676,20 @@
       </c>
       <c r="J15" s="2" t="inlineStr">
         <is>
-          <t>REDUCIR 19%</t>
+          <t>AUMENTAR 19%</t>
         </is>
       </c>
       <c r="K15" s="3" t="n">
         <v>1</v>
       </c>
       <c r="L15" s="3" t="n">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="M15" s="6" t="n">
-        <v>3.75</v>
+        <v>0</v>
       </c>
       <c r="N15" s="4" t="n">
-        <v>2.25</v>
+        <v>0</v>
       </c>
       <c r="O15" s="7" t="inlineStr">
         <is>
@@ -1697,10 +1697,10 @@
         </is>
       </c>
       <c r="P15" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q15" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R15" s="2" t="n">
         <v>0</v>
@@ -1712,10 +1712,10 @@
         <v>1</v>
       </c>
       <c r="U15" s="8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" hidden="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
           <t>9401020010</t>
@@ -1764,13 +1764,13 @@
         <v>1</v>
       </c>
       <c r="L16" s="3" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="M16" s="6" t="n">
-        <v>1.9</v>
+        <v>0</v>
       </c>
       <c r="N16" s="4" t="n">
-        <v>1.14</v>
+        <v>0</v>
       </c>
       <c r="O16" s="7" t="inlineStr">
         <is>
@@ -1778,10 +1778,10 @@
         </is>
       </c>
       <c r="P16" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q16" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R16" s="2" t="n">
         <v>0</v>
@@ -1793,10 +1793,10 @@
         <v>0</v>
       </c>
       <c r="U16" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" hidden="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
           <t>9401020010</t>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">15CM     </t>
+          <t xml:space="preserve">26CM     </t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
@@ -1826,10 +1826,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="4" t="n">
-        <v>0.58</v>
+        <v>1.25</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>0.23</v>
+        <v>0.5</v>
       </c>
       <c r="I17" s="5" t="inlineStr">
         <is>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="J17" s="2" t="inlineStr">
         <is>
-          <t>AUMENTAR 19%</t>
+          <t>REDUCIR 19%</t>
         </is>
       </c>
       <c r="K17" s="3" t="n">
@@ -1848,10 +1848,10 @@
         <v>0</v>
       </c>
       <c r="M17" s="6" t="n">
-        <v>1.72</v>
+        <v>0</v>
       </c>
       <c r="N17" s="4" t="n">
-        <v>1.03</v>
+        <v>0</v>
       </c>
       <c r="O17" s="7" t="inlineStr">
         <is>
@@ -1859,10 +1859,10 @@
         </is>
       </c>
       <c r="P17" s="3" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q17" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R17" s="2" t="n">
         <v>0</v>
@@ -1874,7 +1874,7 @@
         <v>1</v>
       </c>
       <c r="U17" s="8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1929,10 +1929,10 @@
         <v>0</v>
       </c>
       <c r="M18" s="6" t="n">
-        <v>12.6</v>
+        <v>9.449999999999999</v>
       </c>
       <c r="N18" s="4" t="n">
-        <v>7.56</v>
+        <v>5.67</v>
       </c>
       <c r="O18" s="7" t="inlineStr">
         <is>
@@ -1940,10 +1940,10 @@
         </is>
       </c>
       <c r="P18" s="3" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Q18" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R18" s="2" t="n">
         <v>0</v>
@@ -1955,10 +1955,10 @@
         <v>26</v>
       </c>
       <c r="U18" s="8" t="n">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" hidden="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
           <t>9401050006</t>
@@ -2010,10 +2010,10 @@
         <v>0</v>
       </c>
       <c r="M19" s="6" t="n">
-        <v>9.550000000000001</v>
+        <v>0</v>
       </c>
       <c r="N19" s="4" t="n">
-        <v>5.73</v>
+        <v>0</v>
       </c>
       <c r="O19" s="7" t="inlineStr">
         <is>
@@ -2021,10 +2021,10 @@
         </is>
       </c>
       <c r="P19" s="3" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q19" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R19" s="2" t="n">
         <v>0</v>
@@ -2036,10 +2036,10 @@
         <v>0</v>
       </c>
       <c r="U19" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" hidden="1">
       <c r="A20" s="2" t="inlineStr">
         <is>
           <t>9401070015</t>
@@ -2091,10 +2091,10 @@
         <v>0</v>
       </c>
       <c r="M20" s="6" t="n">
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="N20" s="4" t="n">
-        <v>2.88</v>
+        <v>0</v>
       </c>
       <c r="O20" s="7" t="inlineStr">
         <is>
@@ -2102,10 +2102,10 @@
         </is>
       </c>
       <c r="P20" s="3" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="Q20" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R20" s="2" t="n">
         <v>0</v>
@@ -2117,10 +2117,10 @@
         <v>0</v>
       </c>
       <c r="U20" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" hidden="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
           <t>9201050008</t>
@@ -2172,10 +2172,10 @@
         <v>0</v>
       </c>
       <c r="M21" s="6" t="n">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="N21" s="4" t="n">
-        <v>55.2</v>
+        <v>0</v>
       </c>
       <c r="O21" s="7" t="inlineStr">
         <is>
@@ -2183,25 +2183,25 @@
         </is>
       </c>
       <c r="P21" s="3" t="n">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="Q21" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R21" s="2" t="n">
         <v>0</v>
       </c>
       <c r="S21" s="2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="T21" s="3" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="U21" s="8" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" hidden="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
           <t>9201050009</t>
@@ -2253,10 +2253,10 @@
         <v>0</v>
       </c>
       <c r="M22" s="6" t="n">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="N22" s="4" t="n">
-        <v>19.8</v>
+        <v>0</v>
       </c>
       <c r="O22" s="7" t="inlineStr">
         <is>
@@ -2264,25 +2264,25 @@
         </is>
       </c>
       <c r="P22" s="3" t="n">
-        <v>0</v>
+        <v>214</v>
       </c>
       <c r="Q22" s="3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R22" s="2" t="n">
         <v>0</v>
       </c>
       <c r="S22" s="2" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T22" s="3" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="U22" s="8" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" hidden="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
           <t>9201050013</t>
@@ -2334,10 +2334,10 @@
         <v>0</v>
       </c>
       <c r="M23" s="6" t="n">
-        <v>547.5</v>
+        <v>0</v>
       </c>
       <c r="N23" s="4" t="n">
-        <v>328.5</v>
+        <v>0</v>
       </c>
       <c r="O23" s="7" t="inlineStr">
         <is>
@@ -2345,10 +2345,10 @@
         </is>
       </c>
       <c r="P23" s="3" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="Q23" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R23" s="2" t="n">
         <v>0</v>
@@ -2360,10 +2360,10 @@
         <v>0</v>
       </c>
       <c r="U23" s="8" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" hidden="1">
       <c r="A24" s="2" t="inlineStr">
         <is>
           <t>9701010001</t>
@@ -2415,10 +2415,10 @@
         <v>0</v>
       </c>
       <c r="M24" s="6" t="n">
-        <v>48.75</v>
+        <v>0</v>
       </c>
       <c r="N24" s="4" t="n">
-        <v>29.25</v>
+        <v>0</v>
       </c>
       <c r="O24" s="7" t="inlineStr">
         <is>
@@ -2426,10 +2426,10 @@
         </is>
       </c>
       <c r="P24" s="3" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="Q24" s="3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R24" s="2" t="n">
         <v>0</v>
@@ -2441,7 +2441,7 @@
         <v>0</v>
       </c>
       <c r="U24" s="8" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" hidden="1">
@@ -2574,7 +2574,7 @@
         <v>2</v>
       </c>
       <c r="L26" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="6" t="n">
         <v>6.9</v>
@@ -2606,7 +2606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="1">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>9402020004</t>
@@ -2658,10 +2658,10 @@
         <v>0</v>
       </c>
       <c r="M27" s="6" t="n">
-        <v>4.35</v>
+        <v>0</v>
       </c>
       <c r="N27" s="4" t="n">
-        <v>2.61</v>
+        <v>0</v>
       </c>
       <c r="O27" s="7" t="inlineStr">
         <is>
@@ -2669,10 +2669,10 @@
         </is>
       </c>
       <c r="P27" s="3" t="n">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="Q27" s="3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R27" s="2" t="n">
         <v>0</v>
@@ -2684,7 +2684,7 @@
         <v>0</v>
       </c>
       <c r="U27" s="8" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" hidden="1">
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
           <t>9201050010</t>
@@ -2817,13 +2817,13 @@
         <v>1</v>
       </c>
       <c r="L29" s="3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M29" s="6" t="n">
-        <v>18.45</v>
+        <v>0</v>
       </c>
       <c r="N29" s="4" t="n">
-        <v>11.07</v>
+        <v>0</v>
       </c>
       <c r="O29" s="7" t="inlineStr">
         <is>
@@ -2831,22 +2831,22 @@
         </is>
       </c>
       <c r="P29" s="3" t="n">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="Q29" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R29" s="2" t="n">
         <v>0</v>
       </c>
       <c r="S29" s="2" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="T29" s="3" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U29" s="8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -2930,7 +2930,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
           <t>9201050012</t>
@@ -2982,10 +2982,10 @@
         <v>0</v>
       </c>
       <c r="M31" s="6" t="n">
-        <v>68.75</v>
+        <v>0</v>
       </c>
       <c r="N31" s="4" t="n">
-        <v>41.25</v>
+        <v>0</v>
       </c>
       <c r="O31" s="7" t="inlineStr">
         <is>
@@ -2993,10 +2993,10 @@
         </is>
       </c>
       <c r="P31" s="3" t="n">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="Q31" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R31" s="2" t="n">
         <v>0</v>
@@ -3008,7 +3008,7 @@
         <v>0</v>
       </c>
       <c r="U31" s="8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" hidden="1">
@@ -3225,10 +3225,10 @@
         <v>0</v>
       </c>
       <c r="M34" s="6" t="n">
-        <v>65.75</v>
+        <v>32.88</v>
       </c>
       <c r="N34" s="4" t="n">
-        <v>39.45</v>
+        <v>19.73</v>
       </c>
       <c r="O34" s="7" t="inlineStr">
         <is>
@@ -3236,10 +3236,10 @@
         </is>
       </c>
       <c r="P34" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q34" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R34" s="2" t="n">
         <v>0</v>
@@ -3251,10 +3251,10 @@
         <v>0</v>
       </c>
       <c r="U34" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" hidden="1">
       <c r="A35" s="2" t="inlineStr">
         <is>
           <t>9406010020</t>
@@ -3306,10 +3306,10 @@
         <v>0</v>
       </c>
       <c r="M35" s="6" t="n">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="N35" s="4" t="n">
-        <v>32.4</v>
+        <v>0</v>
       </c>
       <c r="O35" s="7" t="inlineStr">
         <is>
@@ -3317,25 +3317,25 @@
         </is>
       </c>
       <c r="P35" s="3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Q35" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R35" s="2" t="n">
         <v>0</v>
       </c>
       <c r="S35" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T35" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" hidden="1">
       <c r="A36" s="2" t="inlineStr">
         <is>
           <t>9201040033</t>
@@ -3387,10 +3387,10 @@
         <v>0</v>
       </c>
       <c r="M36" s="6" t="n">
-        <v>3.1</v>
+        <v>0</v>
       </c>
       <c r="N36" s="4" t="n">
-        <v>1.86</v>
+        <v>0</v>
       </c>
       <c r="O36" s="7" t="inlineStr">
         <is>
@@ -3398,25 +3398,25 @@
         </is>
       </c>
       <c r="P36" s="3" t="n">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="Q36" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R36" s="2" t="n">
         <v>0</v>
       </c>
       <c r="S36" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="T36" s="3" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U36" s="8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" hidden="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
           <t>9201040034</t>
@@ -3468,10 +3468,10 @@
         <v>0</v>
       </c>
       <c r="M37" s="6" t="n">
-        <v>16.8</v>
+        <v>0</v>
       </c>
       <c r="N37" s="4" t="n">
-        <v>10.08</v>
+        <v>0</v>
       </c>
       <c r="O37" s="7" t="inlineStr">
         <is>
@@ -3479,10 +3479,10 @@
         </is>
       </c>
       <c r="P37" s="3" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="Q37" s="3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="R37" s="2" t="n">
         <v>0</v>
@@ -3494,10 +3494,10 @@
         <v>6</v>
       </c>
       <c r="U37" s="8" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" hidden="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
           <t>9303080010</t>
@@ -3549,10 +3549,10 @@
         <v>0</v>
       </c>
       <c r="M38" s="6" t="n">
-        <v>74.75</v>
+        <v>0</v>
       </c>
       <c r="N38" s="4" t="n">
-        <v>44.85</v>
+        <v>0</v>
       </c>
       <c r="O38" s="7" t="inlineStr">
         <is>
@@ -3560,10 +3560,10 @@
         </is>
       </c>
       <c r="P38" s="3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q38" s="3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R38" s="2" t="n">
         <v>0</v>
@@ -3575,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="U38" s="8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39"/>
@@ -3593,7 +3593,7 @@
         </is>
       </c>
       <c r="C41" s="5" t="n">
-        <v>130</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42">
@@ -3614,7 +3614,7 @@
       </c>
       <c r="C43" s="5" t="inlineStr">
         <is>
-          <t>2319.42€</t>
+          <t>1271.48€</t>
         </is>
       </c>
     </row>
@@ -3713,7 +3713,7 @@
         </is>
       </c>
       <c r="C52" s="5" t="n">
-        <v>0</v>
+        <v>-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>